<commit_message>
stage 1 yuan's final
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="19395" windowHeight="6930"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19395" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,17 +16,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>OpenMP</t>
+    <t>Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>MPI</t>
+    <t>OpenMP(24thread)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Size</t>
+    <t>MPI(24thread)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPI(12thread)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenMP(12thread)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,6 +92,630 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.18151E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8945900000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38669100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4509300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.4981900000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20616599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.428645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8755700000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4039700000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0221899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52067799999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3525200000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4611199999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.18701E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52618399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1389699999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="61766272"/>
+        <c:axId val="63635840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="61766272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63635840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63635840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61766272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-CN"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Performance: Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> vs graph size</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8988407699037606E-2"/>
+          <c:y val="0.25789512903946943"/>
+          <c:w val="0.62565048118985123"/>
+          <c:h val="0.5453038244036531"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OpenMP(12thread)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.18151E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8945900000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38669100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4509300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OpenMP(24thread)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7.4981900000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20616599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.428645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8755700000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI(12thread)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4039700000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0221899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52067799999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3525200000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MPI(24thread)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4611199999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.18701E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52618399999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1389699999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="88409600"/>
+        <c:axId val="88411136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88409600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t> of vertices</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.69746631671041115"/>
+              <c:y val="0.84968330062843089"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88411136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="88411136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>running</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t> Time (t)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.2222222222222215E-2"/>
+              <c:y val="0.12701723010175778"/>
+            </c:manualLayout>
+          </c:layout>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88409600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,63 +1003,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>2000</v>
-      </c>
-      <c r="C1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2.8755700000000002</v>
-      </c>
-      <c r="C2">
-        <v>0.428645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>5.1389699999999996</v>
-      </c>
-      <c r="C3">
-        <v>0.52618399999999999</v>
-      </c>
-    </row>
-  </sheetData>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>200</v>
+      </c>
+      <c r="C1">
+        <v>500</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+      <c r="E1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2.18151E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.8945900000000001E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.38669100000000001</v>
+      </c>
+      <c r="E2">
+        <v>2.4509300000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>7.4981900000000004E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.20616599999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.428645</v>
+      </c>
+      <c r="E3">
+        <v>2.8755700000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.4039700000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.0221899999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.52067799999999997</v>
+      </c>
+      <c r="E4">
+        <v>4.3525200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3.4611199999999998E-3</v>
+      </c>
+      <c r="C5">
+        <v>4.18701E-2</v>
+      </c>
+      <c r="D5">
+        <v>0.52618399999999999</v>
+      </c>
+      <c r="E5">
+        <v>5.1389699999999996</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>